<commit_message>
Weekly Adventures Blog Post
</commit_message>
<xml_diff>
--- a/Tools/Generation/Blogging System/Blogging.xlsx
+++ b/Tools/Generation/Blogging System/Blogging.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -44,15 +44,25 @@
   </si>
   <si>
     <t xml:space="preserve">Hello_World.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekly Adventures: Verilog 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekly Adventures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekly_Adventures/2021_05_01.md</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -133,7 +143,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -151,6 +161,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -171,13 +185,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -205,6 +219,20 @@
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>44201.9993055556</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>